<commit_message>
aggiunto tecnologia al file excel
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/installed_capacity/IT-north.xlsx
+++ b/dati_casoStudioItalia/installed_capacity/IT-north.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\installed_capacity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FC19CE1-D975-45B8-9DF4-E2A898848B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65137124-FD13-4E78-BF25-89838DFD88BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-8232" windowWidth="30936" windowHeight="16896" xr2:uid="{4560A6D6-A81C-4D8A-A766-7F07FF6EC7DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4560A6D6-A81C-4D8A-A766-7F07FF6EC7DA}"/>
   </bookViews>
   <sheets>
     <sheet name="time_series" sheetId="1" r:id="rId1"/>
@@ -94,8 +94,66 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Bertoni, L. (Luca)</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{61AF37C6-C02F-46C2-BF19-6D6C4AB2BE4A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bertoni, L. (Luca):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tutti I tipi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{7503DF7E-78BC-4040-ADD1-07DF7BC36C4B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Bertoni, L. (Luca):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sia onshore che offshore</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>hour</t>
   </si>
@@ -119,6 +177,12 @@
   </si>
   <si>
     <t>GasTurbine_simple</t>
+  </si>
+  <si>
+    <t>Photovoltaic</t>
+  </si>
+  <si>
+    <t>Wind_Turbine</t>
   </si>
 </sst>
 </file>
@@ -505,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D9EC3D-3A8C-4C1F-B563-3F4E569D5ADC}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -570,10 +634,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFEE08B-B211-4D4C-AFA9-54AD1D7ACD66}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFEE08B-B211-4D4C-AFA9-54AD1D7ACD66}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -600,7 +666,18 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>